<commit_message>
changes for parsing amount efficiently
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,7 +533,7 @@
       <c r="F4" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="2" t="n">
         <v>45772</v>
       </c>
       <c r="B5" t="inlineStr">
@@ -557,6 +557,264 @@
       <c r="F5" t="inlineStr">
         <is>
           <t>veg fried rice in lunch</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>-27277</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>200</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>April 1825</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>14:47:48</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>soya chap at nearby restaurant</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>40</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14:50:02</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>cold drink</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>46011</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Gym</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$1,200</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>December 2025</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14:52:28</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>gym fees</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>14:54:24</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>tea</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>tea</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$20,000,000</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>14:55:12</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>chill</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>14:55:59</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>playing games in mall</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>14:57:12</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>momos</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>45144</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>75</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>August 2023</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>15:00:05</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>cap</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>45772</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2500</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>15:01:12</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>protien powder</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
added some extra featrues, but was not able to completely implement ask using llm(many errors were there)
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,22 +448,22 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Category</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Amount</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Month</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Time</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -474,347 +474,477 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45772</v>
+        <v>45773</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+          <t>01:49:36</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">surf excel </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45772</v>
+        <v>45773</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>other</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>01:50:16</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>555</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>lunch with friends</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45772</v>
+        <v>45775</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Helpful Assistant Tasks</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>60</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+          <t>01:50:40</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>30</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>bisleri for Abhinav</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>01:51:09</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>food</t>
         </is>
       </c>
-      <c r="C5" t="n">
-        <v>99</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
+      <c r="D5" t="n">
+        <v>60</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>14:26:21</t>
+          <t>April 2025</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>veg fried rice in lunch</t>
+          <t>beetroor juice - me and anupam</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>-27277</v>
+        <v>45916</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>food</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>200</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>April 1825</t>
-        </is>
+          <t>01:51:25</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>120</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>14:47:48</t>
+          <t>September 2025</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>soya chap at nearby restaurant</t>
+          <t>cap - black color</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>food</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>40</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
+          <t>01:53:28</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>14:50:02</t>
+          <t>April 2025</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>cold drink</t>
+          <t>handkerchief</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>46011</v>
+        <v>45774</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Gym</t>
+          <t>02:01:48</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$1,200</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>December 2025</t>
-        </is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>44</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>14:52:28</t>
+          <t>April 2025</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>gym fees</t>
+          <t>ate momos</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>02:05:00</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>food</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
+      <c r="D9" t="n">
+        <v>60</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14:54:24</t>
+          <t>April 2025</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>tea</t>
+          <t>spring roll</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45772</v>
+        <v>45770</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>tea</t>
+          <t>02:08:56</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>$20,000,000</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>23</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>14:55:12</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr"/>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>pepsi</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45772</v>
+        <v>45774</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>chill</t>
+          <t>02:09:14</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
+          <t xml:space="preserve">food </t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>25</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>14:55:59</t>
+          <t>April 2025</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>playing games in mall</t>
+          <t>kellogese chocos</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45772</v>
+        <v>58532</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>02:09:25</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>food</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
+      <c r="D12" t="n">
+        <v>60</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>14:57:12</t>
+          <t>April 2060</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>momos</t>
+          <t>milk</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45144</v>
+        <v>45774</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>clothing</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>75</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>August 2023</t>
-        </is>
+          <t>02:11:09</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>technology</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>2800</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>15:00:05</t>
+          <t>April 2025</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>cap</t>
+          <t>earphones - realme air buds 6</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
-        <v>45772</v>
+      <c r="A14" s="2" t="n">
+        <v>45774</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>02:11:31</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>travel</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>103</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>to mausi house</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>45774</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>02:11:54</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>technology</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1500</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>mouse brought</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>45774</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>02:13:31</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>technology</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>899</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mobile recharge 3 months </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>55610</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>02:45:54</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>food</t>
         </is>
       </c>
-      <c r="C14" t="n">
-        <v>2500</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>April 2025</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>15:01:12</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>protien powder</t>
+      <c r="D17" t="n">
+        <v>52</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>April 2052</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>bananas + paneer</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>45774</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>02:47:23</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>56</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>cocktail</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ask query not working via agent, so did some basic query hardcoding for ask functionality impelmentation
</commit_message>
<xml_diff>
--- a/expenses.xlsx
+++ b/expenses.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -921,7 +921,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="2" t="n">
         <v>45774</v>
       </c>
       <c r="B18" t="inlineStr">
@@ -945,6 +945,118 @@
       <c r="F18" t="inlineStr">
         <is>
           <t>cocktail</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>10:54:19</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>297</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>late night fasos wraps and Dew ( 247 + 50 )</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>13:02:42</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>juice</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>50</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>beetroot + sugarcane juice (20 rs for Abhinav)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>13:05:38</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>20</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>excel surf</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>45775</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>16:18:46</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>bill</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>April 2025</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>electricity bil</t>
         </is>
       </c>
     </row>

</xml_diff>